<commit_message>
Add insertionSort raw data and excel
</commit_message>
<xml_diff>
--- a/raw_data/bucketSort/bucket_sort.xlsx
+++ b/raw_data/bucketSort/bucket_sort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/bucketSort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67B40005-E2E6-0F45-8CF2-820656AA04BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816BDBA-5ADA-D24D-8CF8-24F4431451AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{8D324202-4F98-7642-A210-9E325A65A7CA}"/>
+    <workbookView xWindow="10860" yWindow="460" windowWidth="14660" windowHeight="14700" xr2:uid="{8D324202-4F98-7642-A210-9E325A65A7CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="list_size_with_csv" localSheetId="0">Sheet1!$C$1:$FP$1</definedName>
     <definedName name="running_seconds_with_csv" localSheetId="0">Sheet1!$C$2:$FP$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{E82A69F6-DB9B-3848-8A8F-7594D6AD4AC0}" name="list_size_with_csv" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/insertionSort/list_size_with_csv.csv" decimal="," thousands="." semicolon="1">
+    <textPr sourceFile="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/insertionSort/list_size_with_csv.csv" decimal="," thousands="." semicolon="1">
       <textFields count="171">
         <textField/>
         <textField/>
@@ -208,7 +208,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{2A07AA79-4296-D745-AC18-6D378782C2D5}" name="running_seconds_with_csv" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/insertionSort/running_seconds_with_csv.csv" decimal="," thousands="." semicolon="1">
+    <textPr sourceFile="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/insertionSort/running_seconds_with_csv.csv" decimal="," thousands="." semicolon="1">
       <textFields count="171">
         <textField/>
         <textField/>
@@ -400,10 +400,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,8 +436,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,11 +457,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="running_seconds_with_csv" connectionId="2" xr16:uid="{B5CC2FD4-A0AE-654F-B6D2-E7E7E2697232}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="list_size_with_csv" connectionId="1" xr16:uid="{4FC18C08-E0E7-6A45-87CB-6BB339CD4245}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="list_size_with_csv" connectionId="1" xr16:uid="{4FC18C08-E0E7-6A45-87CB-6BB339CD4245}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="running_seconds_with_csv" connectionId="2" xr16:uid="{B5CC2FD4-A0AE-654F-B6D2-E7E7E2697232}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -753,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A59BCAF-7D88-EE49-8062-A71F4812D467}">
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B171"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="D175" sqref="B175:D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,7 +772,7 @@
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="22" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -2077,7 +2085,7 @@
         <v>138598955</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>3276800</v>
       </c>
@@ -2085,7 +2093,7 @@
         <v>127234497</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>6553600</v>
       </c>
@@ -2093,7 +2101,7 @@
         <v>108975688</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>6553600</v>
       </c>
@@ -2101,7 +2109,7 @@
         <v>176051778</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>6553600</v>
       </c>
@@ -2109,7 +2117,7 @@
         <v>126148874</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>6553600</v>
       </c>
@@ -2117,7 +2125,7 @@
         <v>163705276</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>6553600</v>
       </c>
@@ -2125,7 +2133,7 @@
         <v>173232748</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>6553600</v>
       </c>
@@ -2133,7 +2141,7 @@
         <v>157458158</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>6553600</v>
       </c>
@@ -2141,7 +2149,7 @@
         <v>156586867</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>6553600</v>
       </c>
@@ -2149,7 +2157,7 @@
         <v>171321532</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>6553600</v>
       </c>
@@ -2157,12 +2165,27 @@
         <v>214478110</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>6553600</v>
       </c>
       <c r="B171">
         <v>137491108</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>79802410</v>
+      </c>
+      <c r="C175">
+        <v>137491108</v>
+      </c>
+      <c r="D175">
+        <f>B175-C175</f>
+        <v>-57688698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add priority queue all data, and bucketlist 2nd test
</commit_message>
<xml_diff>
--- a/raw_data/bucketSort/bucket_sort.xlsx
+++ b/raw_data/bucketSort/bucket_sort.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/bucketSort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816BDBA-5ADA-D24D-8CF8-24F4431451AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D777A4-2D50-D043-8638-B115ACF71C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="460" windowWidth="14660" windowHeight="14700" xr2:uid="{8D324202-4F98-7642-A210-9E325A65A7CA}"/>
+    <workbookView xWindow="1960" yWindow="460" windowWidth="23560" windowHeight="14700" activeTab="1" xr2:uid="{8D324202-4F98-7642-A210-9E325A65A7CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="list_size_with_csv" localSheetId="0">Sheet1!$C$1:$FP$1</definedName>
-    <definedName name="running_seconds_with_csv" localSheetId="0">Sheet1!$C$2:$FP$2</definedName>
+    <definedName name="list_size_with_csv" localSheetId="1">Sheet1!$C$1:$FP$1</definedName>
+    <definedName name="nano_time_2" localSheetId="0">Sheet2!$A$1:$FO$1</definedName>
+    <definedName name="running_seconds_with_csv" localSheetId="1">Sheet1!$C$2:$FP$2</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -207,7 +209,184 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{2A07AA79-4296-D745-AC18-6D378782C2D5}" name="running_seconds_with_csv" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{BFC4CD37-38BF-1D4B-90DE-F4AE080F9F2D}" name="nano_time_2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/bucketSort/nano_time_2.csv" decimal="," thousands="." semicolon="1">
+      <textFields count="171">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{2A07AA79-4296-D745-AC18-6D378782C2D5}" name="running_seconds_with_csv" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Keegan/Documents/School/HBO_ICT/Jaar_2/Datastructures/Practicum_opdrachten/Assignment_2/Datastructures_assignment_2/raw_data/insertionSort/running_seconds_with_csv.csv" decimal="," thousands="." semicolon="1">
       <textFields count="171">
         <textField/>
@@ -388,12 +567,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>LIST AMOUNT</t>
   </si>
   <si>
-    <t>RUNNING TIME</t>
+    <t>RUNNING TIME All-in first bucket</t>
+  </si>
+  <si>
+    <t>RUNNING TIME evenly spread bucket</t>
   </si>
 </sst>
 </file>
@@ -436,9 +618,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,11 +642,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="nano_time_2" connectionId="2" xr16:uid="{B5CB0F9B-E3E0-8A4E-97AD-F2E3D8411624}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="list_size_with_csv" connectionId="1" xr16:uid="{4FC18C08-E0E7-6A45-87CB-6BB339CD4245}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="running_seconds_with_csv" connectionId="2" xr16:uid="{B5CC2FD4-A0AE-654F-B6D2-E7E7E2697232}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="running_seconds_with_csv" connectionId="3" xr16:uid="{B5CC2FD4-A0AE-654F-B6D2-E7E7E2697232}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -760,17 +949,564 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFA2BD8-9AFD-A94A-B32F-A1CA633AA3B1}">
+  <dimension ref="A1:FN1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:FN1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="33" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="147" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="148" max="149" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="150" max="155" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="156" max="157" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="158" max="165" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="166" max="168" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="169" max="170" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:170" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>21385696</v>
+      </c>
+      <c r="B1">
+        <v>69233</v>
+      </c>
+      <c r="C1">
+        <v>57784</v>
+      </c>
+      <c r="D1">
+        <v>75134</v>
+      </c>
+      <c r="E1">
+        <v>102345</v>
+      </c>
+      <c r="F1">
+        <v>123252</v>
+      </c>
+      <c r="G1">
+        <v>156198</v>
+      </c>
+      <c r="H1">
+        <v>194313</v>
+      </c>
+      <c r="I1">
+        <v>243766</v>
+      </c>
+      <c r="J1">
+        <v>283102</v>
+      </c>
+      <c r="K1">
+        <v>373611</v>
+      </c>
+      <c r="L1">
+        <v>440987</v>
+      </c>
+      <c r="M1">
+        <v>645479</v>
+      </c>
+      <c r="N1">
+        <v>589455</v>
+      </c>
+      <c r="O1">
+        <v>712984</v>
+      </c>
+      <c r="P1">
+        <v>797814</v>
+      </c>
+      <c r="Q1">
+        <v>32831334</v>
+      </c>
+      <c r="R1">
+        <v>2770161</v>
+      </c>
+      <c r="S1">
+        <v>1315074</v>
+      </c>
+      <c r="T1">
+        <v>1576713</v>
+      </c>
+      <c r="U1">
+        <v>1782803</v>
+      </c>
+      <c r="V1">
+        <v>2023525</v>
+      </c>
+      <c r="W1">
+        <v>1805548</v>
+      </c>
+      <c r="X1">
+        <v>2143795</v>
+      </c>
+      <c r="Y1">
+        <v>2054358</v>
+      </c>
+      <c r="Z1">
+        <v>6461163</v>
+      </c>
+      <c r="AA1">
+        <v>7736097</v>
+      </c>
+      <c r="AB1">
+        <v>3149283</v>
+      </c>
+      <c r="AC1">
+        <v>2703794</v>
+      </c>
+      <c r="AD1">
+        <v>5925348</v>
+      </c>
+      <c r="AE1">
+        <v>2985938</v>
+      </c>
+      <c r="AF1">
+        <v>3077910</v>
+      </c>
+      <c r="AG1">
+        <v>3528261</v>
+      </c>
+      <c r="AH1">
+        <v>54409891</v>
+      </c>
+      <c r="AI1">
+        <v>12060727</v>
+      </c>
+      <c r="AJ1">
+        <v>8578253</v>
+      </c>
+      <c r="AK1">
+        <v>24182131</v>
+      </c>
+      <c r="AL1">
+        <v>7746891</v>
+      </c>
+      <c r="AM1">
+        <v>10990552</v>
+      </c>
+      <c r="AN1">
+        <v>15175429</v>
+      </c>
+      <c r="AO1">
+        <v>21984835</v>
+      </c>
+      <c r="AP1">
+        <v>8145291</v>
+      </c>
+      <c r="AQ1">
+        <v>7238811</v>
+      </c>
+      <c r="AR1">
+        <v>31443124</v>
+      </c>
+      <c r="AS1">
+        <v>10654199</v>
+      </c>
+      <c r="AT1">
+        <v>17201766</v>
+      </c>
+      <c r="AU1">
+        <v>15660289</v>
+      </c>
+      <c r="AV1">
+        <v>32568224</v>
+      </c>
+      <c r="AW1">
+        <v>24264093</v>
+      </c>
+      <c r="AX1">
+        <v>20988342</v>
+      </c>
+      <c r="AY1">
+        <v>26078240</v>
+      </c>
+      <c r="AZ1">
+        <v>23555763</v>
+      </c>
+      <c r="BA1">
+        <v>52933718</v>
+      </c>
+      <c r="BB1">
+        <v>25040337</v>
+      </c>
+      <c r="BC1">
+        <v>10079832</v>
+      </c>
+      <c r="BD1">
+        <v>15080645</v>
+      </c>
+      <c r="BE1">
+        <v>13726537</v>
+      </c>
+      <c r="BF1">
+        <v>14238959</v>
+      </c>
+      <c r="BG1">
+        <v>19440012</v>
+      </c>
+      <c r="BH1">
+        <v>14592800</v>
+      </c>
+      <c r="BI1">
+        <v>13637970</v>
+      </c>
+      <c r="BJ1">
+        <v>12285671</v>
+      </c>
+      <c r="BK1">
+        <v>28104332</v>
+      </c>
+      <c r="BL1">
+        <v>22979961</v>
+      </c>
+      <c r="BM1">
+        <v>29628724</v>
+      </c>
+      <c r="BN1">
+        <v>83317375</v>
+      </c>
+      <c r="BO1">
+        <v>17368600</v>
+      </c>
+      <c r="BP1">
+        <v>32168266</v>
+      </c>
+      <c r="BQ1">
+        <v>33995928</v>
+      </c>
+      <c r="BR1">
+        <v>34303493</v>
+      </c>
+      <c r="BS1">
+        <v>49430597</v>
+      </c>
+      <c r="BT1">
+        <v>70077043</v>
+      </c>
+      <c r="BU1">
+        <v>24211363</v>
+      </c>
+      <c r="BV1">
+        <v>41769228</v>
+      </c>
+      <c r="BW1">
+        <v>25521259</v>
+      </c>
+      <c r="BX1">
+        <v>33609534</v>
+      </c>
+      <c r="BY1">
+        <v>24952052</v>
+      </c>
+      <c r="BZ1">
+        <v>26216821</v>
+      </c>
+      <c r="CA1">
+        <v>35096031</v>
+      </c>
+      <c r="CB1">
+        <v>27131119</v>
+      </c>
+      <c r="CC1">
+        <v>59760084</v>
+      </c>
+      <c r="CD1">
+        <v>24429068</v>
+      </c>
+      <c r="CE1">
+        <v>51600210</v>
+      </c>
+      <c r="CF1">
+        <v>58583616</v>
+      </c>
+      <c r="CG1">
+        <v>79061569</v>
+      </c>
+      <c r="CH1">
+        <v>51639934</v>
+      </c>
+      <c r="CI1">
+        <v>46706414</v>
+      </c>
+      <c r="CJ1">
+        <v>44862821</v>
+      </c>
+      <c r="CK1">
+        <v>39448343</v>
+      </c>
+      <c r="CL1">
+        <v>67749000</v>
+      </c>
+      <c r="CM1">
+        <v>51613110</v>
+      </c>
+      <c r="CN1">
+        <v>54296920</v>
+      </c>
+      <c r="CO1">
+        <v>37575851</v>
+      </c>
+      <c r="CP1">
+        <v>55213317</v>
+      </c>
+      <c r="CQ1">
+        <v>49410488</v>
+      </c>
+      <c r="CR1">
+        <v>33274395</v>
+      </c>
+      <c r="CS1">
+        <v>35421742</v>
+      </c>
+      <c r="CT1">
+        <v>42631670</v>
+      </c>
+      <c r="CU1">
+        <v>32633605</v>
+      </c>
+      <c r="CV1">
+        <v>41985998</v>
+      </c>
+      <c r="CW1">
+        <v>44319344</v>
+      </c>
+      <c r="CX1">
+        <v>35986654</v>
+      </c>
+      <c r="CY1">
+        <v>45377132</v>
+      </c>
+      <c r="CZ1">
+        <v>42087822</v>
+      </c>
+      <c r="DA1">
+        <v>39965480</v>
+      </c>
+      <c r="DB1">
+        <v>49717578</v>
+      </c>
+      <c r="DC1">
+        <v>43351454</v>
+      </c>
+      <c r="DD1">
+        <v>49785199</v>
+      </c>
+      <c r="DE1">
+        <v>51109482</v>
+      </c>
+      <c r="DF1">
+        <v>58944923</v>
+      </c>
+      <c r="DG1">
+        <v>51647512</v>
+      </c>
+      <c r="DH1">
+        <v>52893786</v>
+      </c>
+      <c r="DI1">
+        <v>60102853</v>
+      </c>
+      <c r="DJ1">
+        <v>43689945</v>
+      </c>
+      <c r="DK1">
+        <v>57867121</v>
+      </c>
+      <c r="DL1">
+        <v>71524902</v>
+      </c>
+      <c r="DM1">
+        <v>59120170</v>
+      </c>
+      <c r="DN1">
+        <v>58100981</v>
+      </c>
+      <c r="DO1">
+        <v>61969096</v>
+      </c>
+      <c r="DP1">
+        <v>77983558</v>
+      </c>
+      <c r="DQ1">
+        <v>56375373</v>
+      </c>
+      <c r="DR1">
+        <v>62857468</v>
+      </c>
+      <c r="DS1">
+        <v>57174196</v>
+      </c>
+      <c r="DT1">
+        <v>62779273</v>
+      </c>
+      <c r="DU1">
+        <v>60668777</v>
+      </c>
+      <c r="DV1">
+        <v>62884925</v>
+      </c>
+      <c r="DW1">
+        <v>60238243</v>
+      </c>
+      <c r="DX1">
+        <v>63015251</v>
+      </c>
+      <c r="DY1">
+        <v>57304064</v>
+      </c>
+      <c r="DZ1">
+        <v>61064511</v>
+      </c>
+      <c r="EA1">
+        <v>56629290</v>
+      </c>
+      <c r="EB1">
+        <v>70427514</v>
+      </c>
+      <c r="EC1">
+        <v>64324645</v>
+      </c>
+      <c r="ED1">
+        <v>60553831</v>
+      </c>
+      <c r="EE1">
+        <v>66053540</v>
+      </c>
+      <c r="EF1">
+        <v>66995414</v>
+      </c>
+      <c r="EG1">
+        <v>64224834</v>
+      </c>
+      <c r="EH1">
+        <v>67528995</v>
+      </c>
+      <c r="EI1">
+        <v>77868145</v>
+      </c>
+      <c r="EJ1">
+        <v>77059385</v>
+      </c>
+      <c r="EK1">
+        <v>70848916</v>
+      </c>
+      <c r="EL1">
+        <v>76834406</v>
+      </c>
+      <c r="EM1">
+        <v>79383452</v>
+      </c>
+      <c r="EN1">
+        <v>62888278</v>
+      </c>
+      <c r="EO1">
+        <v>64409470</v>
+      </c>
+      <c r="EP1">
+        <v>73401547</v>
+      </c>
+      <c r="EQ1">
+        <v>74367674</v>
+      </c>
+      <c r="ER1">
+        <v>158276092</v>
+      </c>
+      <c r="ES1">
+        <v>101252852</v>
+      </c>
+      <c r="ET1">
+        <v>70872625</v>
+      </c>
+      <c r="EU1">
+        <v>83955189</v>
+      </c>
+      <c r="EV1">
+        <v>81773628</v>
+      </c>
+      <c r="EW1">
+        <v>74574822</v>
+      </c>
+      <c r="EX1">
+        <v>86295646</v>
+      </c>
+      <c r="EY1">
+        <v>84171607</v>
+      </c>
+      <c r="EZ1">
+        <v>167772438</v>
+      </c>
+      <c r="FA1">
+        <v>119368063</v>
+      </c>
+      <c r="FB1">
+        <v>84014722</v>
+      </c>
+      <c r="FC1">
+        <v>92726745</v>
+      </c>
+      <c r="FD1">
+        <v>87765280</v>
+      </c>
+      <c r="FE1">
+        <v>97746571</v>
+      </c>
+      <c r="FF1">
+        <v>88138261</v>
+      </c>
+      <c r="FG1">
+        <v>89608790</v>
+      </c>
+      <c r="FH1">
+        <v>92987336</v>
+      </c>
+      <c r="FI1">
+        <v>95520135</v>
+      </c>
+      <c r="FJ1">
+        <v>101674209</v>
+      </c>
+      <c r="FK1">
+        <v>106835878</v>
+      </c>
+      <c r="FL1">
+        <v>107523638</v>
+      </c>
+      <c r="FM1">
+        <v>96496953</v>
+      </c>
+      <c r="FN1">
+        <v>94672980</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A59BCAF-7D88-EE49-8062-A71F4812D467}">
   <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="D175" sqref="B175:D175"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -805,1284 +1541,1764 @@
     <col min="155" max="170" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
         <v>7170847</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>21385696</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
       <c r="B3">
         <v>109796</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>69233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
       <c r="B4">
         <v>60548</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>57784</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>100</v>
       </c>
       <c r="B5">
         <v>80132</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>75134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>100</v>
       </c>
       <c r="B6">
         <v>105897</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>102345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>100</v>
       </c>
       <c r="B7">
         <v>138937</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>123252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
       <c r="B8">
         <v>173421</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>156198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
       <c r="B9">
         <v>213048</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>194313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
       <c r="B10">
         <v>274409</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>243766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
       <c r="B11">
         <v>318980</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>283102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>200</v>
       </c>
       <c r="B12">
         <v>466275</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>373611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>200</v>
       </c>
       <c r="B13">
         <v>583784</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>440987</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>200</v>
       </c>
       <c r="B14">
         <v>842673</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>645479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>200</v>
       </c>
       <c r="B15">
         <v>791574</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>589455</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>200</v>
       </c>
       <c r="B16">
         <v>674997</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>712984</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>200</v>
       </c>
       <c r="B17">
         <v>818045</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>797814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>200</v>
       </c>
       <c r="B18">
         <v>1535338</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>32831334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>200</v>
       </c>
       <c r="B19">
         <v>2159127</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>2770161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>200</v>
       </c>
       <c r="B20">
         <v>1051156</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>1315074</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>200</v>
       </c>
       <c r="B21">
         <v>3078882</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>1576713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>400</v>
       </c>
       <c r="B22">
         <v>1779599</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>1782803</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>400</v>
       </c>
       <c r="B23">
         <v>1397985</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>2023525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>400</v>
       </c>
       <c r="B24">
         <v>32517068</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>1805548</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>400</v>
       </c>
       <c r="B25">
         <v>7302115</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>2143795</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>400</v>
       </c>
       <c r="B26">
         <v>4594112</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>2054358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>400</v>
       </c>
       <c r="B27">
         <v>2328670</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>6461163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>400</v>
       </c>
       <c r="B28">
         <v>4744875</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>7736097</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>400</v>
       </c>
       <c r="B29">
         <v>20613640</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>3149283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>400</v>
       </c>
       <c r="B30">
         <v>3155189</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>2703794</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>400</v>
       </c>
       <c r="B31">
         <v>2704479</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>5925348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>800</v>
       </c>
       <c r="B32">
         <v>3007122</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>2985938</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>800</v>
       </c>
       <c r="B33">
         <v>28458893</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>3077910</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>800</v>
       </c>
       <c r="B34">
         <v>19149615</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>3528261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>800</v>
       </c>
       <c r="B35">
         <v>8246449</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>54409891</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>800</v>
       </c>
       <c r="B36">
         <v>8077125</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>12060727</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>800</v>
       </c>
       <c r="B37">
         <v>39043043</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>8578253</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>800</v>
       </c>
       <c r="B38">
         <v>16380558</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>24182131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>800</v>
       </c>
       <c r="B39">
         <v>6524679</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>7746891</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>800</v>
       </c>
       <c r="B40">
         <v>4906803</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>10990552</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>800</v>
       </c>
       <c r="B41">
         <v>5461827</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>15175429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1600</v>
       </c>
       <c r="B42">
         <v>5876051</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>21984835</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1600</v>
       </c>
       <c r="B43">
         <v>6232019</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>8145291</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1600</v>
       </c>
       <c r="B44">
         <v>9902938</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>7238811</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1600</v>
       </c>
       <c r="B45">
         <v>6035008</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>31443124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1600</v>
       </c>
       <c r="B46">
         <v>77090252</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>10654199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1600</v>
       </c>
       <c r="B47">
         <v>9613336</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>17201766</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1600</v>
       </c>
       <c r="B48">
         <v>9007016</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>15660289</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1600</v>
       </c>
       <c r="B49">
         <v>40350181</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>32568224</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1600</v>
       </c>
       <c r="B50">
         <v>86442247</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>24264093</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1600</v>
       </c>
       <c r="B51">
         <v>38300712</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>20988342</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3200</v>
       </c>
       <c r="B52">
         <v>12255644</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>26078240</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3200</v>
       </c>
       <c r="B53">
         <v>33162094</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>23555763</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3200</v>
       </c>
       <c r="B54">
         <v>95925991</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>52933718</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3200</v>
       </c>
       <c r="B55">
         <v>19442751</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>25040337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3200</v>
       </c>
       <c r="B56">
         <v>18479123</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>10079832</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3200</v>
       </c>
       <c r="B57">
         <v>17464762</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>15080645</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3200</v>
       </c>
       <c r="B58">
         <v>13821548</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>13726537</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>3200</v>
       </c>
       <c r="B59">
         <v>83153065</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>14238959</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>3200</v>
       </c>
       <c r="B60">
         <v>11313166</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>19440012</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>3200</v>
       </c>
       <c r="B61">
         <v>51486429</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <v>14592800</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6400</v>
       </c>
       <c r="B62">
         <v>68117857</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <v>13637970</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>6400</v>
       </c>
       <c r="B63">
         <v>44409208</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>12285671</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>6400</v>
       </c>
       <c r="B64">
         <v>22405580</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>28104332</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>6400</v>
       </c>
       <c r="B65">
         <v>17345567</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>22979961</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>6400</v>
       </c>
       <c r="B66">
         <v>28538470</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>29628724</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6400</v>
       </c>
       <c r="B67">
         <v>24002433</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>83317375</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>6400</v>
       </c>
       <c r="B68">
         <v>31278139</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <v>17368600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>6400</v>
       </c>
       <c r="B69">
         <v>19316259</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <v>32168266</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>6400</v>
       </c>
       <c r="B70">
         <v>42644114</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <v>33995928</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>6400</v>
       </c>
       <c r="B71">
         <v>34200579</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <v>34303493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>12800</v>
       </c>
       <c r="B72">
         <v>67367514</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <v>49430597</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>12800</v>
       </c>
       <c r="B73">
         <v>51711880</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73">
+        <v>70077043</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>12800</v>
       </c>
       <c r="B74">
         <v>31354430</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74">
+        <v>24211363</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>12800</v>
       </c>
       <c r="B75">
         <v>60710064</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>41769228</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>12800</v>
       </c>
       <c r="B76">
         <v>21491665</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76">
+        <v>25521259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>12800</v>
       </c>
       <c r="B77">
         <v>22366730</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <v>33609534</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>12800</v>
       </c>
       <c r="B78">
         <v>31673940</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <v>24952052</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>12800</v>
       </c>
       <c r="B79">
         <v>34424909</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <v>26216821</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>12800</v>
       </c>
       <c r="B80">
         <v>31533272</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <v>35096031</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>12800</v>
       </c>
       <c r="B81">
         <v>22467899</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <v>27131119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>25600</v>
       </c>
       <c r="B82">
         <v>32715365</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>59760084</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>25600</v>
       </c>
       <c r="B83">
         <v>22489257</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>24429068</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>25600</v>
       </c>
       <c r="B84">
         <v>29007304</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>51600210</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>25600</v>
       </c>
       <c r="B85">
         <v>30984051</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>58583616</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>25600</v>
       </c>
       <c r="B86">
         <v>43889353</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <v>79061569</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>25600</v>
       </c>
       <c r="B87">
         <v>99433307</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87">
+        <v>51639934</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>25600</v>
       </c>
       <c r="B88">
         <v>33133626</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <v>46706414</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>25600</v>
       </c>
       <c r="B89">
         <v>62499487</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89">
+        <v>44862821</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>25600</v>
       </c>
       <c r="B90">
         <v>34961150</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90">
+        <v>39448343</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>25600</v>
       </c>
       <c r="B91">
         <v>45977498</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>67749000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>51200</v>
       </c>
       <c r="B92">
         <v>33296735</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92">
+        <v>51613110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>51200</v>
       </c>
       <c r="B93">
         <v>57140219</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93">
+        <v>54296920</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>51200</v>
       </c>
       <c r="B94">
         <v>83446354</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94">
+        <v>37575851</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>51200</v>
       </c>
       <c r="B95">
         <v>66728197</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95">
+        <v>55213317</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>51200</v>
       </c>
       <c r="B96">
         <v>60882882</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96">
+        <v>49410488</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>51200</v>
       </c>
       <c r="B97">
         <v>57775820</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97">
+        <v>33274395</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>51200</v>
       </c>
       <c r="B98">
         <v>72755010</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98">
+        <v>35421742</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>51200</v>
       </c>
       <c r="B99">
         <v>35116906</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99">
+        <v>42631670</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>51200</v>
       </c>
       <c r="B100">
         <v>43865603</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100">
+        <v>32633605</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>51200</v>
       </c>
       <c r="B101">
         <v>51194981</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C101">
+        <v>41985998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>102400</v>
       </c>
       <c r="B102">
         <v>41181610</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C102">
+        <v>44319344</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102400</v>
       </c>
       <c r="B103">
         <v>78304037</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C103">
+        <v>35986654</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102400</v>
       </c>
       <c r="B104">
         <v>64727348</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C104">
+        <v>45377132</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>102400</v>
       </c>
       <c r="B105">
         <v>66338765</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C105">
+        <v>42087822</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>102400</v>
       </c>
       <c r="B106">
         <v>45575256</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C106">
+        <v>39965480</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>102400</v>
       </c>
       <c r="B107">
         <v>54676547</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C107">
+        <v>49717578</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>102400</v>
       </c>
       <c r="B108">
         <v>53387253</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C108">
+        <v>43351454</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>102400</v>
       </c>
       <c r="B109">
         <v>85236489</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C109">
+        <v>49785199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>102400</v>
       </c>
       <c r="B110">
         <v>48313628</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C110">
+        <v>51109482</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>102400</v>
       </c>
       <c r="B111">
         <v>71531706</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C111">
+        <v>58944923</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>204800</v>
       </c>
       <c r="B112">
         <v>71994946</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C112">
+        <v>51647512</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>204800</v>
       </c>
       <c r="B113">
         <v>77953586</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C113">
+        <v>52893786</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>204800</v>
       </c>
       <c r="B114">
         <v>74446964</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C114">
+        <v>60102853</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>204800</v>
       </c>
       <c r="B115">
         <v>85762711</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C115">
+        <v>43689945</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>204800</v>
       </c>
       <c r="B116">
         <v>60964453</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C116">
+        <v>57867121</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>204800</v>
       </c>
       <c r="B117">
         <v>51279498</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C117">
+        <v>71524902</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>204800</v>
       </c>
       <c r="B118">
         <v>60417003</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C118">
+        <v>59120170</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>204800</v>
       </c>
       <c r="B119">
         <v>79159802</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C119">
+        <v>58100981</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>204800</v>
       </c>
       <c r="B120">
         <v>77933066</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C120">
+        <v>61969096</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>204800</v>
       </c>
       <c r="B121">
         <v>66479706</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C121">
+        <v>77983558</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>409600</v>
       </c>
       <c r="B122">
         <v>113964510</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C122">
+        <v>56375373</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>409600</v>
       </c>
       <c r="B123">
         <v>85675762</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C123">
+        <v>62857468</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>409600</v>
       </c>
       <c r="B124">
         <v>99322563</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C124">
+        <v>57174196</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>409600</v>
       </c>
       <c r="B125">
         <v>68036163</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C125">
+        <v>62779273</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>409600</v>
       </c>
       <c r="B126">
         <v>74195607</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C126">
+        <v>60668777</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>409600</v>
       </c>
       <c r="B127">
         <v>61878214</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C127">
+        <v>62884925</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>409600</v>
       </c>
       <c r="B128">
         <v>186694753</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C128">
+        <v>60238243</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>409600</v>
       </c>
       <c r="B129">
         <v>118065148</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C129">
+        <v>63015251</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>409600</v>
       </c>
       <c r="B130">
         <v>101150280</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C130">
+        <v>57304064</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>409600</v>
       </c>
       <c r="B131">
         <v>91139001</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C131">
+        <v>61064511</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>819200</v>
       </c>
       <c r="B132">
         <v>87619923</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C132">
+        <v>56629290</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>819200</v>
       </c>
       <c r="B133">
         <v>80563576</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C133">
+        <v>70427514</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>819200</v>
       </c>
       <c r="B134">
         <v>84022343</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C134">
+        <v>64324645</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>819200</v>
       </c>
       <c r="B135">
         <v>132493224</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C135">
+        <v>60553831</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>819200</v>
       </c>
       <c r="B136">
         <v>70567480</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C136">
+        <v>66053540</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>819200</v>
       </c>
       <c r="B137">
         <v>106115924</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C137">
+        <v>66995414</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>819200</v>
       </c>
       <c r="B138">
         <v>118311320</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C138">
+        <v>64224834</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>819200</v>
       </c>
       <c r="B139">
         <v>130521667</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C139">
+        <v>67528995</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>819200</v>
       </c>
       <c r="B140">
         <v>106900319</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140">
+        <v>77868145</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>819200</v>
       </c>
       <c r="B141">
         <v>88758818</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C141">
+        <v>77059385</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1638400</v>
       </c>
       <c r="B142">
         <v>171001311</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C142">
+        <v>70848916</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1638400</v>
       </c>
       <c r="B143">
         <v>146183914</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C143">
+        <v>76834406</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1638400</v>
       </c>
       <c r="B144">
         <v>97725730</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C144">
+        <v>79383452</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>1638400</v>
       </c>
       <c r="B145">
         <v>145930646</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C145">
+        <v>62888278</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>1638400</v>
       </c>
       <c r="B146">
         <v>137277031</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C146">
+        <v>64409470</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1638400</v>
       </c>
       <c r="B147">
         <v>196333770</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C147">
+        <v>73401547</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1638400</v>
       </c>
       <c r="B148">
         <v>88221160</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C148">
+        <v>74367674</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>1638400</v>
       </c>
       <c r="B149">
         <v>89480697</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C149">
+        <v>158276092</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>1638400</v>
       </c>
       <c r="B150">
         <v>89310090</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C150">
+        <v>101252852</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1638400</v>
       </c>
       <c r="B151">
         <v>94485066</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C151">
+        <v>70872625</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>3276800</v>
       </c>
       <c r="B152">
         <v>112596281</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C152">
+        <v>83955189</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>3276800</v>
       </c>
       <c r="B153">
         <v>80680976</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C153">
+        <v>81773628</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>3276800</v>
       </c>
       <c r="B154">
         <v>103021307</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C154">
+        <v>74574822</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>3276800</v>
       </c>
       <c r="B155">
         <v>99877556</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C155">
+        <v>86295646</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>3276800</v>
       </c>
       <c r="B156">
         <v>111161818</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C156">
+        <v>84171607</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>3276800</v>
       </c>
       <c r="B157">
         <v>112829446</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C157">
+        <v>167772438</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>3276800</v>
       </c>
       <c r="B158">
         <v>126522015</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C158">
+        <v>119368063</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>3276800</v>
       </c>
       <c r="B159">
         <v>192299997</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C159">
+        <v>84014722</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>3276800</v>
       </c>
       <c r="B160">
         <v>138598955</v>
+      </c>
+      <c r="C160">
+        <v>92726745</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -2092,6 +3308,9 @@
       <c r="B161">
         <v>127234497</v>
       </c>
+      <c r="C161">
+        <v>87765280</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -2100,6 +3319,9 @@
       <c r="B162">
         <v>108975688</v>
       </c>
+      <c r="C162">
+        <v>97746571</v>
+      </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -2108,6 +3330,9 @@
       <c r="B163">
         <v>176051778</v>
       </c>
+      <c r="C163">
+        <v>88138261</v>
+      </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -2116,6 +3341,9 @@
       <c r="B164">
         <v>126148874</v>
       </c>
+      <c r="C164">
+        <v>89608790</v>
+      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165">
@@ -2124,6 +3352,9 @@
       <c r="B165">
         <v>163705276</v>
       </c>
+      <c r="C165">
+        <v>92987336</v>
+      </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166">
@@ -2132,6 +3363,9 @@
       <c r="B166">
         <v>173232748</v>
       </c>
+      <c r="C166">
+        <v>95520135</v>
+      </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167">
@@ -2140,6 +3374,9 @@
       <c r="B167">
         <v>157458158</v>
       </c>
+      <c r="C167">
+        <v>101674209</v>
+      </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168">
@@ -2148,6 +3385,9 @@
       <c r="B168">
         <v>156586867</v>
       </c>
+      <c r="C168">
+        <v>106835878</v>
+      </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169">
@@ -2156,6 +3396,9 @@
       <c r="B169">
         <v>171321532</v>
       </c>
+      <c r="C169">
+        <v>107523638</v>
+      </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170">
@@ -2164,6 +3407,9 @@
       <c r="B170">
         <v>214478110</v>
       </c>
+      <c r="C170">
+        <v>96496953</v>
+      </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171">
@@ -2171,6 +3417,9 @@
       </c>
       <c r="B171">
         <v>137491108</v>
+      </c>
+      <c r="C171">
+        <v>94672980</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>